<commit_message>
Send email - reset password
</commit_message>
<xml_diff>
--- a/documents/Outline.xlsx
+++ b/documents/Outline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\TestOnline\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B4DCD1E-3042-496B-B92C-311564ABF8B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C32CC3D-A947-48DC-B6FA-CD167FC0E9F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="145">
   <si>
     <t>URL</t>
   </si>
@@ -426,6 +426,36 @@
   </si>
   <si>
     <t>Response</t>
+  </si>
+  <si>
+    <t>sendEmail</t>
+  </si>
+  <si>
+    <t>Tạo slug và gửi mail cho người dùng</t>
+  </si>
+  <si>
+    <t>Đặt lại mật khẩu dựa trên slug</t>
+  </si>
+  <si>
+    <t>/user/sendEmail</t>
+  </si>
+  <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>newPassword</t>
+  </si>
+  <si>
+    <t>updatePassword</t>
+  </si>
+  <si>
+    <t>/user/updatePassword/:slug</t>
+  </si>
+  <si>
+    <t>msg, newUser</t>
+  </si>
+  <si>
+    <t>email</t>
   </si>
 </sst>
 </file>
@@ -964,13 +994,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE889BF-D16E-469E-A614-B33F6C18E738}">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1212,321 +1242,317 @@
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="20"/>
-    </row>
-    <row r="14" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
-        <v>114</v>
+        <v>141</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="20"/>
+    </row>
+    <row r="16" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F15" s="2"/>
-      <c r="H15" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>78</v>
       </c>
       <c r="F16" s="2"/>
-      <c r="G16" s="3" t="s">
-        <v>96</v>
-      </c>
+      <c r="G16" s="2"/>
       <c r="H16" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="H17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="1:9" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="I17" s="2"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="20"/>
-    </row>
-    <row r="19" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="20"/>
+    </row>
+    <row r="21" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="10" t="s">
+      <c r="G21" s="2"/>
+      <c r="H21" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="I19" s="2"/>
-    </row>
-    <row r="20" spans="1:9" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="11" t="s">
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="1:9" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A22" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="3" t="s">
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="H22" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A21" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F21" s="2"/>
-      <c r="G21" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>78</v>
       </c>
       <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="G23" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="H23" s="2" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>78</v>
       </c>
       <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
+      <c r="G24" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="H24" s="2" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>78</v>
       </c>
       <c r="F25" s="2"/>
-      <c r="G25" s="3" t="s">
-        <v>104</v>
-      </c>
+      <c r="G25" s="2"/>
       <c r="H25" s="2" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>78</v>
@@ -1534,170 +1560,170 @@
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>78</v>
       </c>
       <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>111</v>
+      <c r="G27" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
-        <v>81</v>
+        <v>126</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E28" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="I28" s="2"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="20"/>
-    </row>
-    <row r="30" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
-        <v>128</v>
+        <v>81</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
-      <c r="G30" s="3" t="s">
+      <c r="G30" s="2"/>
+      <c r="H30" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I30" s="2"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="20"/>
+    </row>
+    <row r="32" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="H32" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A31" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F31" s="2"/>
-      <c r="G31" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>78</v>
       </c>
       <c r="F33" s="2"/>
-      <c r="G33" s="2" t="s">
-        <v>103</v>
+      <c r="G33" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I33" s="2" t="s">
         <v>108</v>
@@ -1705,62 +1731,114 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>78</v>
       </c>
       <c r="F34" s="2"/>
-      <c r="G34" s="2" t="s">
-        <v>102</v>
-      </c>
+      <c r="G34" s="2"/>
       <c r="H34" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I34" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A37" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2" t="s">
+      <c r="E37" s="2"/>
+      <c r="F37" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2" t="s">
+      <c r="G37" s="2"/>
+      <c r="H37" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="I35" s="2"/>
+      <c r="I37" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A29:I29"/>
+    <mergeCell ref="A31:I31"/>
     <mergeCell ref="A8:I8"/>
-    <mergeCell ref="A18:I18"/>
+    <mergeCell ref="A20:I20"/>
     <mergeCell ref="A4:I4"/>
     <mergeCell ref="E1:G1"/>
-    <mergeCell ref="A13:I13"/>
+    <mergeCell ref="A15:I15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Response answers for submit
</commit_message>
<xml_diff>
--- a/documents/Outline.xlsx
+++ b/documents/Outline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\TestOnline\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C32CC3D-A947-48DC-B6FA-CD167FC0E9F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{780A92AE-71D4-41DE-8E15-0E05092527A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="146">
   <si>
     <t>URL</t>
   </si>
@@ -284,9 +284,6 @@
     <t>msg, removeExam</t>
   </si>
   <si>
-    <t>msg, score</t>
-  </si>
-  <si>
     <t>msg, updateExam</t>
   </si>
   <si>
@@ -456,6 +453,12 @@
   </si>
   <si>
     <t>email</t>
+  </si>
+  <si>
+    <t>answers</t>
+  </si>
+  <si>
+    <t>msg, score,answers</t>
   </si>
 </sst>
 </file>
@@ -997,10 +1000,10 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomRight" activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1036,7 +1039,7 @@
       <c r="F1" s="22"/>
       <c r="G1" s="23"/>
       <c r="H1" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>4</v>
@@ -1155,7 +1158,7 @@
     </row>
     <row r="9" spans="1:9" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>38</v>
@@ -1178,7 +1181,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>36</v>
@@ -1199,7 +1202,7 @@
     </row>
     <row r="11" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>38</v>
@@ -1222,7 +1225,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>36</v>
@@ -1243,21 +1246,21 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>76</v>
@@ -1266,26 +1269,26 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I14" s="2"/>
     </row>
@@ -1304,7 +1307,7 @@
     </row>
     <row r="16" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>36</v>
@@ -1324,12 +1327,12 @@
         <v>79</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>38</v>
@@ -1351,7 +1354,7 @@
     </row>
     <row r="18" spans="1:9" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>39</v>
@@ -1367,18 +1370,18 @@
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>80</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>38</v>
@@ -1391,10 +1394,10 @@
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>82</v>
@@ -1416,7 +1419,7 @@
     </row>
     <row r="21" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>36</v>
@@ -1429,7 +1432,7 @@
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="10" t="s">
@@ -1439,7 +1442,7 @@
     </row>
     <row r="22" spans="1:9" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>38</v>
@@ -1453,18 +1456,18 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>83</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>40</v>
@@ -1480,18 +1483,18 @@
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>85</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>41</v>
@@ -1507,18 +1510,18 @@
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>79</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>36</v>
@@ -1538,12 +1541,12 @@
         <v>79</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>38</v>
@@ -1558,17 +1561,19 @@
         <v>78</v>
       </c>
       <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
+      <c r="G26" s="2" t="s">
+        <v>144</v>
+      </c>
       <c r="H26" s="2" t="s">
-        <v>87</v>
+        <v>145</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>39</v>
@@ -1584,18 +1589,18 @@
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>41</v>
@@ -1615,12 +1620,12 @@
         <v>86</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>36</v>
@@ -1637,10 +1642,10 @@
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
@@ -1679,7 +1684,7 @@
     </row>
     <row r="32" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>38</v>
@@ -1693,18 +1698,18 @@
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>39</v>
@@ -1720,18 +1725,18 @@
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>41</v>
@@ -1748,15 +1753,15 @@
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>40</v>
@@ -1772,18 +1777,18 @@
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>41</v>
@@ -1799,18 +1804,18 @@
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>36</v>
@@ -1823,11 +1828,11 @@
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I37" s="2"/>
     </row>

</xml_diff>